<commit_message>
Updated chrome app tests
</commit_message>
<xml_diff>
--- a/data/metadata/SRA-metadata-15476171-processed-ok.xlsx
+++ b/data/metadata/SRA-metadata-15476171-processed-ok.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam.rivers/Documents/tamipami/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C83C923B-0719-3E4E-B4B1-C8E8342B4225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D8096-3E52-6749-8069-E80F286F0748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44980" yWindow="-4560" windowWidth="38140" windowHeight="16480" xr2:uid="{7E7F4ADA-8DFD-8440-B361-70A37B4CF1D0}"/>
+    <workbookView xWindow="-44840" yWindow="6720" windowWidth="38140" windowHeight="16480" xr2:uid="{7E7F4ADA-8DFD-8440-B361-70A37B4CF1D0}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata-15476171-processed-ok" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1197,9 +1210,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DF4D20-071C-FE49-986E-AE9EF9016EFD}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>